<commit_message>
Added analysis of noise of experimental data and used this to add noise to simulated data
</commit_message>
<xml_diff>
--- a/StreyCats/Broken Feedback Circuit/Broken_Feedback_Circuit_High_Expression_Example.xlsx
+++ b/StreyCats/Broken Feedback Circuit/Broken_Feedback_Circuit_High_Expression_Example.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Strey Lab\Documents\GitHub\Analysis_of_SGC_Simulations\StreyCats\Broken Feedback Circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCDC8E9B-B75D-438A-9B6F-E0E06A6C2D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875F8F4E-708D-4677-89B7-BE6E4563EE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BDFEC2D-7785-4D75-A48D-6701B0246CBC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Broken_Feedback_Circuit_Example" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>